<commit_message>
feat: Add LAP collateral, 5-level approval workflow, collection API, seed data, and comprehensive docs
- Collateral module: 4 models (Collateral, Valuation, Insurance, LegalVerification) with auto-LTV
- Document model enhanced with media_type, section, geo-tagging (11 new fields)
- 5-level LAP approval workflow: Branch → Manager → Regional → Central → Sanctioning Authority
- Collection API: case management, actions, promise-to-pay, escalation rules, dashboard
- Delinquency enhancements: sticky NPA, bucket distribution, trend analysis
- EOD batch service and PAR (Portfolio at Risk) reporting with 60+ variables
- Demo seed data: 10 borrowers, 6 products, 9 applications, 6 accounts, full entity graph
- Comprehensive documentation (39 sections, 1875 lines)
- Detailed 52-slide presentation with module deep-dives
- 453 tests passing across 22 test files

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/LOS_LMS_Module_Statistics.xlsx
+++ b/docs/LOS_LMS_Module_Statistics.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D Drive\LOS LMS\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050DD123-FBA0-4271-81BC-F092BF4C5E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Statistics" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
     <sheet name="Schemas" sheetId="7" r:id="rId7"/>
     <sheet name="New Modules Summary" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -719,8 +725,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -824,13 +830,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -868,7 +882,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -902,6 +916,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -936,9 +951,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1111,18 +1127,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.7265625" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1130,15 +1148,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1146,7 +1164,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1154,7 +1172,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1162,7 +1180,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1170,7 +1188,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1178,7 +1196,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1186,7 +1204,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1200,19 +1218,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="50.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.7265625" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" customWidth="1"/>
+    <col min="3" max="3" width="50.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1223,7 +1241,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -1234,7 +1252,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -1245,7 +1263,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1256,7 +1274,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
@@ -1267,7 +1285,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -1278,7 +1296,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -1289,7 +1307,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
@@ -1300,7 +1318,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
@@ -1311,7 +1329,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -1322,7 +1340,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
@@ -1333,7 +1351,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -1344,7 +1362,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>37</v>
       </c>
@@ -1355,7 +1373,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
@@ -1366,7 +1384,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
@@ -1377,7 +1395,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>43</v>
       </c>
@@ -1388,7 +1406,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>45</v>
       </c>
@@ -1399,7 +1417,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>47</v>
       </c>
@@ -1410,7 +1428,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>49</v>
       </c>
@@ -1421,7 +1439,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>51</v>
       </c>
@@ -1432,7 +1450,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>53</v>
       </c>
@@ -1443,7 +1461,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>55</v>
       </c>
@@ -1454,7 +1472,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>57</v>
       </c>
@@ -1465,7 +1483,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>59</v>
       </c>
@@ -1476,7 +1494,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>61</v>
       </c>
@@ -1487,7 +1505,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>63</v>
       </c>
@@ -1498,7 +1516,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>65</v>
       </c>
@@ -1509,7 +1527,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>67</v>
       </c>
@@ -1520,7 +1538,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>69</v>
       </c>
@@ -1531,7 +1549,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>71</v>
       </c>
@@ -1542,7 +1560,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>73</v>
       </c>
@@ -1553,7 +1571,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>75</v>
       </c>
@@ -1564,7 +1582,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>77</v>
       </c>
@@ -1575,7 +1593,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>79</v>
       </c>
@@ -1586,7 +1604,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
         <v>81</v>
       </c>
@@ -1603,19 +1621,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="55.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.7265625" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" customWidth="1"/>
+    <col min="3" max="3" width="55.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>83</v>
       </c>
@@ -1626,7 +1644,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -1637,7 +1655,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -1648,7 +1666,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
@@ -1659,7 +1677,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -1670,7 +1688,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>89</v>
       </c>
@@ -1681,7 +1699,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
@@ -1692,7 +1710,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -1703,7 +1721,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>27</v>
       </c>
@@ -1714,7 +1732,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>51</v>
       </c>
@@ -1725,7 +1743,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>95</v>
       </c>
@@ -1736,7 +1754,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -1747,7 +1765,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
@@ -1758,7 +1776,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>99</v>
       </c>
@@ -1769,7 +1787,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>101</v>
       </c>
@@ -1780,7 +1798,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>55</v>
       </c>
@@ -1791,7 +1809,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>104</v>
       </c>
@@ -1802,7 +1820,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>106</v>
       </c>
@@ -1813,7 +1831,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>108</v>
       </c>
@@ -1824,7 +1842,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>110</v>
       </c>
@@ -1835,7 +1853,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>65</v>
       </c>
@@ -1846,7 +1864,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>113</v>
       </c>
@@ -1857,7 +1875,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>115</v>
       </c>
@@ -1868,7 +1886,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>117</v>
       </c>
@@ -1879,7 +1897,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>119</v>
       </c>
@@ -1890,7 +1908,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>121</v>
       </c>
@@ -1901,7 +1919,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>123</v>
       </c>
@@ -1912,7 +1930,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>81</v>
       </c>
@@ -1929,19 +1947,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.7265625" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" customWidth="1"/>
+    <col min="3" max="3" width="45.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>126</v>
       </c>
@@ -1952,7 +1970,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>128</v>
       </c>
@@ -1963,7 +1981,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>130</v>
       </c>
@@ -1974,7 +1992,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>132</v>
       </c>
@@ -1985,7 +2003,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>134</v>
       </c>
@@ -1996,7 +2014,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>136</v>
       </c>
@@ -2007,7 +2025,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>138</v>
       </c>
@@ -2018,7 +2036,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>140</v>
       </c>
@@ -2029,7 +2047,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>142</v>
       </c>
@@ -2040,7 +2058,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>143</v>
       </c>
@@ -2051,7 +2069,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>145</v>
       </c>
@@ -2062,7 +2080,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>41</v>
       </c>
@@ -2073,7 +2091,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>148</v>
       </c>
@@ -2084,7 +2102,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>81</v>
       </c>
@@ -2101,19 +2119,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="45.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.7265625" customWidth="1"/>
+    <col min="2" max="3" width="10.7265625" customWidth="1"/>
+    <col min="4" max="4" width="45.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>151</v>
       </c>
@@ -2127,7 +2145,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>154</v>
       </c>
@@ -2141,7 +2159,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>156</v>
       </c>
@@ -2155,7 +2173,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>158</v>
       </c>
@@ -2169,7 +2187,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>160</v>
       </c>
@@ -2183,7 +2201,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>162</v>
       </c>
@@ -2197,7 +2215,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>164</v>
       </c>
@@ -2211,7 +2229,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>166</v>
       </c>
@@ -2225,7 +2243,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>168</v>
       </c>
@@ -2239,7 +2257,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>81</v>
       </c>
@@ -2259,20 +2277,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="50.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.7265625" customWidth="1"/>
+    <col min="2" max="3" width="10.7265625" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" customWidth="1"/>
+    <col min="5" max="5" width="50.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>171</v>
       </c>
@@ -2289,7 +2307,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>174</v>
       </c>
@@ -2306,7 +2324,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>177</v>
       </c>
@@ -2323,7 +2341,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>180</v>
       </c>
@@ -2340,7 +2358,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>183</v>
       </c>
@@ -2357,7 +2375,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>186</v>
       </c>
@@ -2374,7 +2392,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>188</v>
       </c>
@@ -2391,7 +2409,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>191</v>
       </c>
@@ -2408,7 +2426,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>194</v>
       </c>
@@ -2425,7 +2443,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>197</v>
       </c>
@@ -2442,7 +2460,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>200</v>
       </c>
@@ -2459,7 +2477,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>203</v>
       </c>
@@ -2476,7 +2494,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>205</v>
       </c>
@@ -2493,7 +2511,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>81</v>
       </c>
@@ -2516,19 +2534,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.7265625" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" customWidth="1"/>
+    <col min="3" max="3" width="40.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>209</v>
       </c>
@@ -2539,7 +2557,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
@@ -2550,7 +2568,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
@@ -2561,7 +2579,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>59</v>
       </c>
@@ -2572,7 +2590,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>45</v>
       </c>
@@ -2583,7 +2601,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>63</v>
       </c>
@@ -2594,7 +2612,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>69</v>
       </c>
@@ -2605,7 +2623,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>71</v>
       </c>
@@ -2616,7 +2634,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>77</v>
       </c>
@@ -2627,7 +2645,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>79</v>
       </c>
@@ -2638,7 +2656,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>67</v>
       </c>
@@ -2649,7 +2667,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>73</v>
       </c>
@@ -2660,7 +2678,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>47</v>
       </c>
@@ -2671,7 +2689,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>53</v>
       </c>
@@ -2682,7 +2700,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>81</v>
       </c>
@@ -2699,19 +2717,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="50.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7265625" customWidth="1"/>
+    <col min="2" max="3" width="15.7265625" customWidth="1"/>
+    <col min="4" max="4" width="50.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>171</v>
       </c>
@@ -2725,7 +2743,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>200</v>
       </c>
@@ -2739,7 +2757,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>203</v>
       </c>
@@ -2753,7 +2771,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>81</v>
       </c>

</xml_diff>